<commit_message>
Changes `JENIS_TRANSAKSI_KAS` from enumartion into an entity (`JenisTransaksiKas`).
</commit_message>
<xml_diff>
--- a/test/integration/project/data_laba_rugi.xlsx
+++ b/test/integration/project/data_laba_rugi.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="kategorikas" sheetId="50" r:id="rId1"/>
     <sheet name="kategorikas_listjumlahkas" sheetId="51" r:id="rId2"/>
     <sheet name="transaksikas" sheetId="52" r:id="rId3"/>
+    <sheet name="jenistransaksikas" sheetId="53" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -100,6 +101,15 @@
   </si>
   <si>
     <t>tahun</t>
+  </si>
+  <si>
+    <t>jenis_id</t>
+  </si>
+  <si>
+    <t>Dalam Kota</t>
+  </si>
+  <si>
+    <t>Luar Kota</t>
   </si>
 </sst>
 </file>
@@ -487,7 +497,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -635,14 +645,14 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" customWidth="1"/>
     <col min="5" max="5" width="6.140625" customWidth="1"/>
   </cols>
@@ -655,7 +665,7 @@
         <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>17</v>
@@ -672,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D2">
         <v>10000</v>
@@ -689,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="D3">
         <v>12000</v>
@@ -708,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -718,7 +728,7 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -742,7 +752,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
@@ -783,7 +793,7 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F2">
         <v>10000</v>
@@ -815,7 +825,7 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="F3">
         <v>12000</v>
@@ -836,4 +846,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1">
+        <v>41971</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>41971</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add feature to refresh monthly cash balance.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_laba_rugi.xlsx
+++ b/test/integration/project/data_laba_rugi.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="kategorikas" sheetId="50" r:id="rId1"/>
-    <sheet name="kategorikas_listjumlahkas" sheetId="51" r:id="rId2"/>
+    <sheet name="kategorikas_listsaldokas" sheetId="51" r:id="rId2"/>
     <sheet name="transaksikas" sheetId="52" r:id="rId3"/>
     <sheet name="jenistransaksikas" sheetId="53" r:id="rId4"/>
   </sheets>
@@ -644,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -852,7 +852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add `KlaimTambahBayaran` and `KlaimTukarUang`.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_laba_rugi.xlsx
+++ b/test/integration/project/data_laba_rugi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="kategorikas" sheetId="50" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -644,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -718,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -850,10 +850,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -867,7 +867,7 @@
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -889,8 +889,11 @@
       <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -903,8 +906,11 @@
       <c r="G2" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-2</v>
       </c>
@@ -916,6 +922,9 @@
       </c>
       <c r="G3" s="2" t="s">
         <v>29</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow excluding transaction's category in reports.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_laba_rugi.xlsx
+++ b/test/integration/project/data_laba_rugi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788"/>
   </bookViews>
   <sheets>
     <sheet name="kategorikas" sheetId="50" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>id</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Luar Kota</t>
+  </si>
+  <si>
+    <t>dipakaiDiLaporan</t>
   </si>
 </sst>
 </file>
@@ -494,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -510,10 +513,11 @@
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -539,10 +543,13 @@
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -564,8 +571,11 @@
       <c r="I2" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-2</v>
       </c>
@@ -584,11 +594,14 @@
       <c r="H3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-3</v>
       </c>
@@ -607,11 +620,14 @@
       <c r="H4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-4</v>
       </c>
@@ -630,7 +646,10 @@
       <c r="H5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I5" t="b">
+      <c r="I5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -852,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Allow multiple cash accounts.
</commit_message>
<xml_diff>
--- a/test/integration/project/data_laba_rugi.xlsx
+++ b/test/integration/project/data_laba_rugi.xlsx
@@ -4,23 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="14940" windowHeight="7455" tabRatio="788"/>
+    <workbookView xWindow="360" yWindow="450" windowWidth="14940" windowHeight="7395" tabRatio="859" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="kategorikas" sheetId="50" r:id="rId1"/>
-    <sheet name="kategorikas_listsaldokas" sheetId="51" r:id="rId2"/>
-    <sheet name="transaksikas" sheetId="52" r:id="rId3"/>
-    <sheet name="jenistransaksikas" sheetId="53" r:id="rId4"/>
+    <sheet name="kas" sheetId="54" r:id="rId1"/>
+    <sheet name="kategorikas" sheetId="55" r:id="rId2"/>
+    <sheet name="jenistransaksikas" sheetId="53" r:id="rId3"/>
+    <sheet name="periodekas_listtransaksikas" sheetId="59" r:id="rId4"/>
+    <sheet name="periodekas" sheetId="60" r:id="rId5"/>
+    <sheet name="periodekas_jumlahperiodik" sheetId="61" r:id="rId6"/>
   </sheets>
-  <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -46,9 +45,6 @@
     <t>keterangan</t>
   </si>
   <si>
-    <t>nomor</t>
-  </si>
-  <si>
     <t>tanggal</t>
   </si>
   <si>
@@ -70,9 +66,6 @@
     <t>sistem</t>
   </si>
   <si>
-    <t>KategoriKas_id</t>
-  </si>
-  <si>
     <t>saldo</t>
   </si>
   <si>
@@ -85,24 +78,12 @@
     <t>Lain-Lain</t>
   </si>
   <si>
-    <t>TR-001</t>
-  </si>
-  <si>
     <t>unknown</t>
   </si>
   <si>
-    <t>TR-002</t>
-  </si>
-  <si>
     <t>snake</t>
   </si>
   <si>
-    <t>bulan</t>
-  </si>
-  <si>
-    <t>tahun</t>
-  </si>
-  <si>
     <t>jenis_id</t>
   </si>
   <si>
@@ -113,6 +94,33 @@
   </si>
   <si>
     <t>dipakaiDiLaporan</t>
+  </si>
+  <si>
+    <t>Kas Kecil</t>
+  </si>
+  <si>
+    <t>PeriodeKas_id</t>
+  </si>
+  <si>
+    <t>listTransaksiKas_ORDER</t>
+  </si>
+  <si>
+    <t>arsip</t>
+  </si>
+  <si>
+    <t>tanggalMulai</t>
+  </si>
+  <si>
+    <t>tanggalSelesai</t>
+  </si>
+  <si>
+    <t>listPeriodeRiwayat_id</t>
+  </si>
+  <si>
+    <t>listPeriodeRiwayat_ORDER</t>
+  </si>
+  <si>
+    <t>jenisTransaksiKas_id</t>
   </si>
 </sst>
 </file>
@@ -497,10 +505,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2">
+        <v>22000</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
+        <v>41985</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -509,11 +595,11 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -522,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -531,22 +617,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -554,7 +640,7 @@
         <v>-1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4">
         <v>41970</v>
@@ -562,16 +648,16 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2" t="b">
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -580,7 +666,7 @@
         <v>-2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>41970</v>
@@ -588,14 +674,14 @@
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="2" t="b">
-        <v>1</v>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -606,7 +692,7 @@
         <v>-3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>41970</v>
@@ -614,14 +700,14 @@
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="2" t="b">
-        <v>1</v>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="J4" t="b">
         <v>1</v>
@@ -632,7 +718,7 @@
         <v>-4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
         <v>41970</v>
@@ -640,226 +726,17 @@
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="2" t="b">
-        <v>1</v>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>-1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>-1</v>
-      </c>
-      <c r="D2">
-        <v>10000</v>
-      </c>
-      <c r="E2">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>-1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>-2</v>
-      </c>
-      <c r="D3">
-        <v>12000</v>
-      </c>
-      <c r="E3">
-        <v>2014</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>-1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1">
-        <v>41970</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>-1</v>
-      </c>
-      <c r="F2">
-        <v>10000</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="1">
-        <v>41641</v>
-      </c>
-      <c r="M2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>-2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1">
-        <v>41970</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>-2</v>
-      </c>
-      <c r="F3">
-        <v>12000</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="1">
-        <v>41642</v>
-      </c>
-      <c r="M3">
-        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -867,7 +744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -891,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -900,7 +777,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>3</v>
@@ -909,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -917,13 +794,13 @@
         <v>-1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>41971</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H2" t="b">
         <v>1</v>
@@ -934,16 +811,294 @@
         <v>-2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <v>41971</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>10000</v>
+      </c>
+      <c r="G2">
+        <v>10000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>41641</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-1</v>
+      </c>
+      <c r="B3">
+        <v>-2</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>12000</v>
+      </c>
+      <c r="G3">
+        <v>22000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>41642</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>32000</v>
+      </c>
+      <c r="D2">
+        <v>32000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>41640</v>
+      </c>
+      <c r="F2" s="1">
+        <v>41670</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1">
+        <v>41985</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <v>-1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>-1</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>-1</v>
+      </c>
+      <c r="B3">
+        <v>-2</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>12000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>